<commit_message>
Internal Develop to External Develop Sync
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
@@ -6975,12 +6975,6 @@
     <t>exa-bkup</t>
   </si>
   <si>
-    <t>10.113.1.0/28</t>
-  </si>
-  <si>
-    <t>10.113.1.16/28</t>
-  </si>
-  <si>
     <t>VCN::exa-vcn</t>
   </si>
   <si>
@@ -7597,6 +7591,12 @@
   </si>
   <si>
     <t>exa-bkup-rt</t>
+  </si>
+  <si>
+    <t>10.113.0.0/28</t>
+  </si>
+  <si>
+    <t>10.113.0.16/28</t>
   </si>
 </sst>
 </file>
@@ -12645,7 +12645,7 @@
     <row r="1" spans="1:1" ht="15" thickBot="1"/>
     <row r="2" spans="1:1" ht="59.25" customHeight="1" thickBot="1">
       <c r="A2" s="90" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
   </sheetData>
@@ -12658,8 +12658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R502"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A6" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -13310,7 +13310,7 @@
         <v>989</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>993</v>
+        <v>1034</v>
       </c>
       <c r="F13" s="38" t="s">
         <v>51</v>
@@ -13361,7 +13361,7 @@
         <v>992</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>994</v>
+        <v>1035</v>
       </c>
       <c r="F14" s="38" t="s">
         <v>51</v>
@@ -13371,10 +13371,10 @@
       </c>
       <c r="H14" s="38"/>
       <c r="I14" s="38" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="K14" s="38" t="s">
         <v>23</v>
@@ -18708,7 +18708,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="63" customHeight="1">
       <c r="A1" s="111" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>
@@ -19582,7 +19582,7 @@
         <v>79</v>
       </c>
       <c r="K11" s="36" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="L11" s="36"/>
       <c r="M11" s="36"/>
@@ -19595,7 +19595,7 @@
       <c r="P11" s="36"/>
       <c r="Q11" s="36"/>
       <c r="R11" s="36" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="S11" s="36"/>
       <c r="T11" s="36"/>
@@ -19628,7 +19628,7 @@
         <v>79</v>
       </c>
       <c r="K12" s="36" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="L12" s="36"/>
       <c r="M12" s="36"/>
@@ -19641,7 +19641,7 @@
       <c r="P12" s="36"/>
       <c r="Q12" s="36"/>
       <c r="R12" s="36" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="S12" s="36"/>
       <c r="T12" s="36"/>
@@ -20432,7 +20432,7 @@
         <v>79</v>
       </c>
       <c r="K30" s="36" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="L30" s="36"/>
       <c r="M30" s="36"/>
@@ -20445,7 +20445,7 @@
       <c r="P30" s="36"/>
       <c r="Q30" s="36"/>
       <c r="R30" s="36" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="S30" s="36"/>
       <c r="T30" s="36"/>
@@ -20478,7 +20478,7 @@
         <v>79</v>
       </c>
       <c r="K31" s="36" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="L31" s="36"/>
       <c r="M31" s="36"/>
@@ -20491,7 +20491,7 @@
       <c r="P31" s="36"/>
       <c r="Q31" s="36"/>
       <c r="R31" s="36" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="S31" s="36"/>
       <c r="T31" s="36"/>
@@ -20897,7 +20897,7 @@
         <v>988</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E41" s="36" t="s">
         <v>508</v>
@@ -20914,7 +20914,7 @@
         <v>372</v>
       </c>
       <c r="K41" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="L41" s="36"/>
       <c r="M41" s="36"/>
@@ -20927,7 +20927,7 @@
       <c r="P41" s="36"/>
       <c r="Q41" s="36"/>
       <c r="R41" s="36" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="S41" s="36"/>
       <c r="T41" s="36"/>
@@ -20943,7 +20943,7 @@
         <v>988</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E42" s="36" t="s">
         <v>508</v>
@@ -20989,7 +20989,7 @@
         <v>988</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E43" s="36" t="s">
         <v>509</v>
@@ -21004,7 +21004,7 @@
         <v>372</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
@@ -21019,7 +21019,7 @@
       <c r="P43" s="36"/>
       <c r="Q43" s="36"/>
       <c r="R43" s="36" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="S43" s="36"/>
       <c r="T43" s="36"/>
@@ -21035,7 +21035,7 @@
         <v>988</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E44" s="36" t="s">
         <v>509</v>
@@ -21065,7 +21065,7 @@
       <c r="P44" s="36"/>
       <c r="Q44" s="36"/>
       <c r="R44" s="36" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="S44" s="36"/>
       <c r="T44" s="36"/>
@@ -21081,7 +21081,7 @@
         <v>988</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E45" s="36" t="s">
         <v>509</v>
@@ -21096,7 +21096,7 @@
         <v>372</v>
       </c>
       <c r="I45" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="J45" s="36"/>
       <c r="K45" s="36"/>
@@ -21111,7 +21111,7 @@
       <c r="P45" s="36"/>
       <c r="Q45" s="36"/>
       <c r="R45" s="36" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="S45" s="36"/>
       <c r="T45" s="36"/>
@@ -21127,7 +21127,7 @@
         <v>988</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E46" s="36" t="s">
         <v>509</v>
@@ -21157,7 +21157,7 @@
       <c r="P46" s="36"/>
       <c r="Q46" s="36"/>
       <c r="R46" s="36" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="S46" s="36"/>
       <c r="T46" s="36"/>
@@ -21173,7 +21173,7 @@
         <v>988</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E47" s="36" t="s">
         <v>509</v>
@@ -21203,7 +21203,7 @@
       <c r="P47" s="36"/>
       <c r="Q47" s="36"/>
       <c r="R47" s="36" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="S47" s="36"/>
       <c r="T47" s="36"/>
@@ -21219,7 +21219,7 @@
         <v>988</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E48" s="36" t="s">
         <v>509</v>
@@ -21249,7 +21249,7 @@
       <c r="P48" s="36"/>
       <c r="Q48" s="36"/>
       <c r="R48" s="36" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="S48" s="36"/>
       <c r="T48" s="36"/>
@@ -21265,7 +21265,7 @@
         <v>988</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E49" s="36" t="s">
         <v>508</v>
@@ -21282,7 +21282,7 @@
         <v>372</v>
       </c>
       <c r="K49" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="L49" s="36"/>
       <c r="M49" s="36"/>
@@ -21295,7 +21295,7 @@
       <c r="P49" s="36"/>
       <c r="Q49" s="36"/>
       <c r="R49" s="36" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="S49" s="36"/>
       <c r="T49" s="36"/>
@@ -21311,7 +21311,7 @@
         <v>988</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E50" s="36" t="s">
         <v>509</v>
@@ -21341,7 +21341,7 @@
       <c r="P50" s="36"/>
       <c r="Q50" s="36"/>
       <c r="R50" s="36" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="S50" s="36"/>
       <c r="T50" s="36"/>
@@ -21357,7 +21357,7 @@
         <v>988</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E51" s="36" t="s">
         <v>508</v>
@@ -21374,7 +21374,7 @@
         <v>372</v>
       </c>
       <c r="K51" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="L51" s="36"/>
       <c r="M51" s="36"/>
@@ -21387,7 +21387,7 @@
       <c r="P51" s="36"/>
       <c r="Q51" s="36"/>
       <c r="R51" s="36" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="S51" s="36"/>
       <c r="T51" s="36"/>
@@ -21403,7 +21403,7 @@
         <v>988</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E52" s="36" t="s">
         <v>509</v>
@@ -21433,7 +21433,7 @@
       <c r="P52" s="36"/>
       <c r="Q52" s="36"/>
       <c r="R52" s="36" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="S52" s="36"/>
       <c r="T52" s="36"/>
@@ -21449,7 +21449,7 @@
         <v>988</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E53" s="36" t="s">
         <v>509</v>
@@ -21464,7 +21464,7 @@
         <v>372</v>
       </c>
       <c r="I53" s="36" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="J53" s="36"/>
       <c r="K53" s="36"/>
@@ -21479,7 +21479,7 @@
       <c r="P53" s="36"/>
       <c r="Q53" s="36"/>
       <c r="R53" s="36" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="S53" s="36"/>
       <c r="T53" s="36"/>
@@ -21495,7 +21495,7 @@
         <v>988</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="E54" s="36" t="s">
         <v>508</v>
@@ -21512,7 +21512,7 @@
         <v>511</v>
       </c>
       <c r="K54" s="36" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="L54" s="36"/>
       <c r="M54" s="36"/>
@@ -21525,7 +21525,7 @@
       <c r="P54" s="36"/>
       <c r="Q54" s="36"/>
       <c r="R54" s="36" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="S54" s="36"/>
       <c r="T54" s="36"/>
@@ -21925,19 +21925,19 @@
         <v>336</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="G3" s="38" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="I3" s="38" t="s">
         <v>424</v>
       </c>
       <c r="J3" s="88" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="K3" s="38">
         <v>8</v>
@@ -25087,13 +25087,13 @@
         <v>726</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="E4" s="61" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="61" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="G4" s="61"/>
       <c r="H4" s="61" t="s">
@@ -25574,7 +25574,7 @@
         <v>10000</v>
       </c>
       <c r="K4" s="61" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="29">
@@ -25607,7 +25607,7 @@
         <v>10000</v>
       </c>
       <c r="K5" s="61" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="29">
@@ -25634,7 +25634,7 @@
         <v>20000</v>
       </c>
       <c r="K6" s="61" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
   </sheetData>
@@ -25668,7 +25668,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="37" customFormat="1" ht="160" customHeight="1">
       <c r="A1" s="112" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B1" s="113"/>
       <c r="C1" s="113"/>
@@ -25694,13 +25694,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>311</v>
@@ -25715,10 +25715,10 @@
         <v>641</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="L2" s="58" t="s">
         <v>646</v>
@@ -25764,14 +25764,14 @@
         <v>446</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="D4" s="61" t="s">
         <v>671</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="60" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="G4" s="60"/>
       <c r="H4" s="103" t="s">
@@ -32224,7 +32224,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="119.25" customHeight="1">
       <c r="A1" s="112" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B1" s="113"/>
       <c r="C1" s="113"/>
@@ -53231,7 +53231,7 @@
         <v>988</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>489</v>
@@ -53343,14 +53343,14 @@
   <sheetData>
     <row r="1" spans="1:8" ht="222" customHeight="1">
       <c r="A1" s="111" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>
       <c r="D1" s="111"/>
       <c r="E1" s="111"/>
       <c r="F1" s="118" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="G1" s="118"/>
       <c r="H1" s="118"/>
@@ -53456,7 +53456,7 @@
         <v>489</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>559</v>

</xml_diff>

<commit_message>
Updated CIS template with remote-exec example and details
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\cd3_automation_toolkit\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unamachi\Desktop\code\cd3_public\17042023\cd3-automation-toolkit\cd3_automation_toolkit\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B4CB44-52DD-42AF-9A7B-B8ECCC336FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01A5CD8-C10F-495E-9CA3-A2D8AD018DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="1000" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="1252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="1258">
   <si>
     <t>Region</t>
   </si>
@@ -7861,6 +7861,725 @@
     </r>
   </si>
   <si>
+    <t>allow group AnnouncementReaders to read announcements in tenancy</t>
+  </si>
+  <si>
+    <t>allow group AnnouncementReaders to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>allow group AppDevAdmins to read app-catalog-listing in tenancy</t>
+  </si>
+  <si>
+    <t>allow group AppDevAdmins to read instance-images in tenancy</t>
+  </si>
+  <si>
+    <t>allow group AppDevAdmins to read repos in tenancy</t>
+  </si>
+  <si>
+    <t>allow group AppDevAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>allow group AppDevAdmins to read usage-budgets in tenancy</t>
+  </si>
+  <si>
+    <t>allow group AppDevAdmins to read usage-reports in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to inspect all-resources in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read instances in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read load-balancers in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read buckets in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read nat-gateways in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read public-ips in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read file-family in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read instance-configurations in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read network-security-groups in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read resource-availability in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read audit-events in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read users in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read vss-family in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read usage-budgets in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read usage-reports in tenancy</t>
+  </si>
+  <si>
+    <t>allow group Auditors to read data-safe-family in tenancy</t>
+  </si>
+  <si>
+    <t>Policy for Credential Admins group</t>
+  </si>
+  <si>
+    <t>allow group CredAdmins to inspect users in tenancy</t>
+  </si>
+  <si>
+    <t>allow group CredAdmins to inspect groups in tenancy</t>
+  </si>
+  <si>
+    <t>allow group CredAdmins to manage users in tenancy  where any {request.operation = 'ListApiKeys',request.operation = 'ListAuthTokens',request.operation = 'ListCustomerSecretKeys',request.operation = 'UploadApiKey',request.operation = 'DeleteApiKey',request.operation = 'UpdateAuthToken',request.operation = 'CreateAuthToken',request.operation = 'DeleteAuthToken',request.operation = 'CreateSecretKey',request.operation = 'UpdateCustomerSecretKey',request.operation = 'DeleteCustomerSecretKey',request.operation = 'UpdateUserCapabilities'}</t>
+  </si>
+  <si>
+    <t>allow group CredAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>Managed-Services-Policy</t>
+  </si>
+  <si>
+    <t>allow service cloudguard to read all-resources in tenancy</t>
+  </si>
+  <si>
+    <t>allow service cloudguard to use network-security-groups in tenancy</t>
+  </si>
+  <si>
+    <t>allow service osms to read instances in tenancy</t>
+  </si>
+  <si>
+    <t>allow group DatabaseAdmins to read usage-reports in tenancy</t>
+  </si>
+  <si>
+    <t>allow group DatabaseAdmins to read usage-budgets in tenancy</t>
+  </si>
+  <si>
+    <t>allow group IAMAdmins to manage policies in tenancy</t>
+  </si>
+  <si>
+    <t>allow group IAMAdmins to manage compartments in tenancy</t>
+  </si>
+  <si>
+    <t>allow group IAMAdmins to manage identity-providers in tenancy where any {request.operation = 'AddIdpgroupMapping', request.operation = 'DeleteIdpgroupMapping'}</t>
+  </si>
+  <si>
+    <t>allow group NetworkAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>allow group NetworkAdmins to read usage-budgets in tenancy</t>
+  </si>
+  <si>
+    <t>allow group NetworkAdmins to read usage-reports in tenancy</t>
+  </si>
+  <si>
+    <t>define tenancy usage-report as ocid1.tenancy.oc1..aaaaaaaaned4fkpkisbwjlr56u7cj63lf3wffbilvqknstgtvzub7vhqkggq</t>
+  </si>
+  <si>
+    <t>allow group CostAdmins to manage usage-report in tenancy</t>
+  </si>
+  <si>
+    <t>allow group CostAdmins to manage usage-budgets  in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to manage tag-namespaces in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to manage tag-defaults in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to manage repos in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to read audit-events in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to read app-catalog-listing in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to read instance-images in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to inspect buckets in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to manage cloudevents-rules in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to manage cloud-guard-family in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to read tenancies in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to read objectstorage-namespaces in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to use cloud-shell in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to read usage-budgets in tenancy</t>
+  </si>
+  <si>
+    <t>allow group SecurityAdmins to read usage-reports in tenancy</t>
+  </si>
+  <si>
+    <t>Shapes</t>
+  </si>
+  <si>
+    <t>DB version</t>
+  </si>
+  <si>
+    <t>DB workload</t>
+  </si>
+  <si>
+    <t>EXA Shapes</t>
+  </si>
+  <si>
+    <t>ADB workload</t>
+  </si>
+  <si>
+    <t>VM.Standard2.1</t>
+  </si>
+  <si>
+    <t>ENTERPRISE_EDITION_EXTREME_PERFORMANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.2.0.4 </t>
+  </si>
+  <si>
+    <t>Exadata.Quarter2.92</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>VM.Standard1.1</t>
+  </si>
+  <si>
+    <t>12.1.0.2</t>
+  </si>
+  <si>
+    <t>DSS</t>
+  </si>
+  <si>
+    <t>Exadata.Half2.184</t>
+  </si>
+  <si>
+    <t>BRING_YOUR_OWN_LICENSE</t>
+  </si>
+  <si>
+    <t>UTF8</t>
+  </si>
+  <si>
+    <t>AR8ADOS710</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>VM.Standard1.2</t>
+  </si>
+  <si>
+    <t>12.2.0.1</t>
+  </si>
+  <si>
+    <t>Exadata.Full2.368</t>
+  </si>
+  <si>
+    <t>AR8ADOS720</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>ENTERPRISE_EDITION_HIGH_PERFORMANCE</t>
+  </si>
+  <si>
+    <t>18.0.0.0</t>
+  </si>
+  <si>
+    <t>Exadata.Quarter1.84</t>
+  </si>
+  <si>
+    <t>AR8APTEC715</t>
+  </si>
+  <si>
+    <t>APEX</t>
+  </si>
+  <si>
+    <t>VM.Standard2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.12.0.0 </t>
+  </si>
+  <si>
+    <t>Exadata.Half1.168</t>
+  </si>
+  <si>
+    <t>AR8ARABICMACS</t>
+  </si>
+  <si>
+    <t>VM.Standard1.4</t>
+  </si>
+  <si>
+    <t>18.13.0.0</t>
+  </si>
+  <si>
+    <t>Exadata.Full1.336</t>
+  </si>
+  <si>
+    <t>AR8ASMO8X</t>
+  </si>
+  <si>
+    <t>VM.Standard1.8</t>
+  </si>
+  <si>
+    <t>18.14.0.0</t>
+  </si>
+  <si>
+    <t>Exadata.Base.48</t>
+  </si>
+  <si>
+    <t>AR8ISO8859P6</t>
+  </si>
+  <si>
+    <t>VM.Standard2.8</t>
+  </si>
+  <si>
+    <t>Exadata.Half3.200</t>
+  </si>
+  <si>
+    <t>AR8MSWIN1256</t>
+  </si>
+  <si>
+    <t>VM.Standard2.16</t>
+  </si>
+  <si>
+    <t>19.10.0.0</t>
+  </si>
+  <si>
+    <t>Exadata.Quater3.100</t>
+  </si>
+  <si>
+    <t>AR8MUSSAD768</t>
+  </si>
+  <si>
+    <t>VM.Standard1.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.11.0.0 </t>
+  </si>
+  <si>
+    <t>Exadata.Full3.400</t>
+  </si>
+  <si>
+    <t>AR8NAFITHA711</t>
+  </si>
+  <si>
+    <t>VM.Standard2.24</t>
+  </si>
+  <si>
+    <t>19.12.0.0</t>
+  </si>
+  <si>
+    <t>Exadata X8M-2</t>
+  </si>
+  <si>
+    <t>AR8NAFITHA721</t>
+  </si>
+  <si>
+    <t>BM.DenseIO1.36</t>
+  </si>
+  <si>
+    <t>21.0.0.0</t>
+  </si>
+  <si>
+    <t>Exadata X9M-2</t>
+  </si>
+  <si>
+    <t>AR8SAKHR706</t>
+  </si>
+  <si>
+    <t>21.3.0.0</t>
+  </si>
+  <si>
+    <t>AR8SAKHR707</t>
+  </si>
+  <si>
+    <t>AZ8ISO8859P9E</t>
+  </si>
+  <si>
+    <t>BG8MSWIN</t>
+  </si>
+  <si>
+    <t>BG8PC437S</t>
+  </si>
+  <si>
+    <t>BLT8CP921</t>
+  </si>
+  <si>
+    <t>BLT8ISO8859P13</t>
+  </si>
+  <si>
+    <t>BLT8MSWIN1257</t>
+  </si>
+  <si>
+    <t>BLT8PC775</t>
+  </si>
+  <si>
+    <t>BN8BSCII</t>
+  </si>
+  <si>
+    <t>CDN8PC863</t>
+  </si>
+  <si>
+    <t>CEL8ISO8859P14</t>
+  </si>
+  <si>
+    <t>CL8ISO8859P5</t>
+  </si>
+  <si>
+    <t>CL8ISOIR111</t>
+  </si>
+  <si>
+    <t>CL8KOI8R</t>
+  </si>
+  <si>
+    <t>CL8KOI8U</t>
+  </si>
+  <si>
+    <t>CL8MACCYRILLICS</t>
+  </si>
+  <si>
+    <t>CL8MSWIN1251</t>
+  </si>
+  <si>
+    <t>EE8ISO8859P2</t>
+  </si>
+  <si>
+    <t>EE8MACCES</t>
+  </si>
+  <si>
+    <t>EE8MACCROATIANS</t>
+  </si>
+  <si>
+    <t>EE8MSWIN1250</t>
+  </si>
+  <si>
+    <t>EE8PC852</t>
+  </si>
+  <si>
+    <t>EL8DEC</t>
+  </si>
+  <si>
+    <t>EL8ISO8859P7</t>
+  </si>
+  <si>
+    <t>EL8MACGREEKS</t>
+  </si>
+  <si>
+    <t>EL8MSWIN1253</t>
+  </si>
+  <si>
+    <t>EL8PC437S</t>
+  </si>
+  <si>
+    <t>EL8PC851</t>
+  </si>
+  <si>
+    <t>EL8PC869</t>
+  </si>
+  <si>
+    <t>ET8MSWIN923</t>
+  </si>
+  <si>
+    <t>HU8ABMOD</t>
+  </si>
+  <si>
+    <t>HU8CWI2</t>
+  </si>
+  <si>
+    <t>IN8ISCII</t>
+  </si>
+  <si>
+    <t>IS8PC861</t>
+  </si>
+  <si>
+    <t>IW8ISO8859P8</t>
+  </si>
+  <si>
+    <t>IW8MACHEBREWS</t>
+  </si>
+  <si>
+    <t>IW8MSWIN1255</t>
+  </si>
+  <si>
+    <t>IW8PC1507</t>
+  </si>
+  <si>
+    <t>JA16EUC</t>
+  </si>
+  <si>
+    <t>JA16EUCTILDE</t>
+  </si>
+  <si>
+    <t>JA16SJIS</t>
+  </si>
+  <si>
+    <t>JA16SJISTILDE</t>
+  </si>
+  <si>
+    <t>JA16VMS</t>
+  </si>
+  <si>
+    <t>KO16KSC5601</t>
+  </si>
+  <si>
+    <t>KO16KSCCS</t>
+  </si>
+  <si>
+    <t>KO16MSWIN949</t>
+  </si>
+  <si>
+    <t>LA8ISO6937</t>
+  </si>
+  <si>
+    <t>LA8PASSPORT</t>
+  </si>
+  <si>
+    <t>LT8MSWIN921</t>
+  </si>
+  <si>
+    <t>LT8PC772</t>
+  </si>
+  <si>
+    <t>LT8PC774</t>
+  </si>
+  <si>
+    <t>LV8PC1117</t>
+  </si>
+  <si>
+    <t>LV8PC8LR</t>
+  </si>
+  <si>
+    <t>LV8RST104090</t>
+  </si>
+  <si>
+    <t>N8PC865</t>
+  </si>
+  <si>
+    <t>NE8ISO8859P10</t>
+  </si>
+  <si>
+    <t>NEE8ISO8859P4</t>
+  </si>
+  <si>
+    <t>RU8BESTA</t>
+  </si>
+  <si>
+    <t>RU8PC855</t>
+  </si>
+  <si>
+    <t>RU8PC866</t>
+  </si>
+  <si>
+    <t>SE8ISO8859P3</t>
+  </si>
+  <si>
+    <t>TH8MACTHAIS</t>
+  </si>
+  <si>
+    <t>TH8TISASCII</t>
+  </si>
+  <si>
+    <t>TR8DEC</t>
+  </si>
+  <si>
+    <t>TR8MACTURKISHS</t>
+  </si>
+  <si>
+    <t>TR8MSWIN1254</t>
+  </si>
+  <si>
+    <t>TR8PC857</t>
+  </si>
+  <si>
+    <t>US7ASCII</t>
+  </si>
+  <si>
+    <t>US8PC437</t>
+  </si>
+  <si>
+    <t>VN8MSWIN1258</t>
+  </si>
+  <si>
+    <t>VN8VN3</t>
+  </si>
+  <si>
+    <t>WE8DEC</t>
+  </si>
+  <si>
+    <t>WE8DG</t>
+  </si>
+  <si>
+    <t>WE8ISO8859P1</t>
+  </si>
+  <si>
+    <t>WE8ISO8859P15</t>
+  </si>
+  <si>
+    <t>WE8ISO8859P9</t>
+  </si>
+  <si>
+    <t>WE8MACROMAN8S</t>
+  </si>
+  <si>
+    <t>WE8MSWIN1252</t>
+  </si>
+  <si>
+    <t>WE8NCR4970</t>
+  </si>
+  <si>
+    <t>WE8NEXTSTEP</t>
+  </si>
+  <si>
+    <t>WE8PC850</t>
+  </si>
+  <si>
+    <t>WE8PC858</t>
+  </si>
+  <si>
+    <t>WE8PC860</t>
+  </si>
+  <si>
+    <t>WE8ROMAN8</t>
+  </si>
+  <si>
+    <t>ZHS16CGB231280</t>
+  </si>
+  <si>
+    <t>ZHS16GBK</t>
+  </si>
+  <si>
+    <t>ZHT16BIG5</t>
+  </si>
+  <si>
+    <t>ZHT16CCDC</t>
+  </si>
+  <si>
+    <t>ZHT16DBT</t>
+  </si>
+  <si>
+    <t>ZHT16HKSCS</t>
+  </si>
+  <si>
+    <t>ZHT16MSWIN950</t>
+  </si>
+  <si>
+    <t>ZHT32EUC</t>
+  </si>
+  <si>
+    <t>ZHT32SOPS</t>
+  </si>
+  <si>
+    <t>ZHT32TRIS</t>
+  </si>
+  <si>
+    <r>
+      <t>"Attached To</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" - Valid format:
+VCN::&lt;vcn_name&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Import DRG Route Distribution Statements"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Valid format: &lt;matchtype&gt;::&lt;type|ocid&gt;::&lt;priority&gt;  Multiple statements are seperated by newline in the same cell(\n is not supported)
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>eg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALL::::1
+       DRG_ATTACHMENT_TYPE::VCN::2
+       DRG_ATTACHMENT_TYPE::IPSEC_TUNNEL::2
+       DRG_ATTACHMENT_TYPE::REMOTE_PEERING_CONNECTION::2
+       DRG_ATTACHMENT_TYPE::VIRTUAL_CIRCUIT::2
+       DRG_ATTACHMENT_ID::&lt;OCID&gt;::3</t>
+    </r>
+  </si>
+  <si>
+    <t>Remote Execute</t>
+  </si>
+  <si>
+    <t>ansible_default</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 </t>
@@ -7973,7 +8692,51 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Leave this field empty if the instance does not need to be launched on dedicated vm host.
+      <t>Leave this field empty if the instance does not need to be launched on dedicated vm host.
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remote Execute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" - To execute script(Ansible/Shell) remotely during provisioning. Format is,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ansible_&lt;script_name&gt; or shell_&lt;script_name&gt; without ext (shell script should be named with *.sh and ansible with *.yaml inside scripts folder within region dir)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -8090,731 +8853,18 @@
       <t xml:space="preserve">
 </t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>allow group AnnouncementReaders to read announcements in tenancy</t>
-  </si>
-  <si>
-    <t>allow group AnnouncementReaders to use cloud-shell in tenancy</t>
-  </si>
-  <si>
-    <t>allow group AppDevAdmins to read app-catalog-listing in tenancy</t>
-  </si>
-  <si>
-    <t>allow group AppDevAdmins to read instance-images in tenancy</t>
-  </si>
-  <si>
-    <t>allow group AppDevAdmins to read repos in tenancy</t>
-  </si>
-  <si>
-    <t>allow group AppDevAdmins to use cloud-shell in tenancy</t>
-  </si>
-  <si>
-    <t>allow group AppDevAdmins to read usage-budgets in tenancy</t>
-  </si>
-  <si>
-    <t>allow group AppDevAdmins to read usage-reports in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to inspect all-resources in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read instances in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read load-balancers in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read buckets in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read nat-gateways in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read public-ips in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read file-family in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read instance-configurations in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read network-security-groups in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read resource-availability in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read audit-events in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to use cloud-shell in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read users in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read vss-family in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read usage-budgets in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read usage-reports in tenancy</t>
-  </si>
-  <si>
-    <t>allow group Auditors to read data-safe-family in tenancy</t>
-  </si>
-  <si>
-    <t>Policy for Credential Admins group</t>
-  </si>
-  <si>
-    <t>allow group CredAdmins to inspect users in tenancy</t>
-  </si>
-  <si>
-    <t>allow group CredAdmins to inspect groups in tenancy</t>
-  </si>
-  <si>
-    <t>allow group CredAdmins to manage users in tenancy  where any {request.operation = 'ListApiKeys',request.operation = 'ListAuthTokens',request.operation = 'ListCustomerSecretKeys',request.operation = 'UploadApiKey',request.operation = 'DeleteApiKey',request.operation = 'UpdateAuthToken',request.operation = 'CreateAuthToken',request.operation = 'DeleteAuthToken',request.operation = 'CreateSecretKey',request.operation = 'UpdateCustomerSecretKey',request.operation = 'DeleteCustomerSecretKey',request.operation = 'UpdateUserCapabilities'}</t>
-  </si>
-  <si>
-    <t>allow group CredAdmins to use cloud-shell in tenancy</t>
-  </si>
-  <si>
-    <t>Managed-Services-Policy</t>
-  </si>
-  <si>
-    <t>allow service cloudguard to read all-resources in tenancy</t>
-  </si>
-  <si>
-    <t>allow service cloudguard to use network-security-groups in tenancy</t>
-  </si>
-  <si>
-    <t>allow service osms to read instances in tenancy</t>
-  </si>
-  <si>
-    <t>allow group DatabaseAdmins to read usage-reports in tenancy</t>
-  </si>
-  <si>
-    <t>allow group DatabaseAdmins to read usage-budgets in tenancy</t>
-  </si>
-  <si>
-    <t>allow group IAMAdmins to manage policies in tenancy</t>
-  </si>
-  <si>
-    <t>allow group IAMAdmins to manage compartments in tenancy</t>
-  </si>
-  <si>
-    <t>allow group IAMAdmins to manage identity-providers in tenancy where any {request.operation = 'AddIdpgroupMapping', request.operation = 'DeleteIdpgroupMapping'}</t>
-  </si>
-  <si>
-    <t>allow group NetworkAdmins to use cloud-shell in tenancy</t>
-  </si>
-  <si>
-    <t>allow group NetworkAdmins to read usage-budgets in tenancy</t>
-  </si>
-  <si>
-    <t>allow group NetworkAdmins to read usage-reports in tenancy</t>
-  </si>
-  <si>
-    <t>define tenancy usage-report as ocid1.tenancy.oc1..aaaaaaaaned4fkpkisbwjlr56u7cj63lf3wffbilvqknstgtvzub7vhqkggq</t>
-  </si>
-  <si>
-    <t>allow group CostAdmins to manage usage-report in tenancy</t>
-  </si>
-  <si>
-    <t>allow group CostAdmins to manage usage-budgets  in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to manage tag-namespaces in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to manage tag-defaults in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to manage repos in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to read audit-events in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to read app-catalog-listing in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to read instance-images in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to inspect buckets in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to manage cloudevents-rules in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to manage cloud-guard-family in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to read tenancies in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to read objectstorage-namespaces in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to use cloud-shell in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to read usage-budgets in tenancy</t>
-  </si>
-  <si>
-    <t>allow group SecurityAdmins to read usage-reports in tenancy</t>
-  </si>
-  <si>
-    <t>Shapes</t>
-  </si>
-  <si>
-    <t>DB version</t>
-  </si>
-  <si>
-    <t>DB workload</t>
-  </si>
-  <si>
-    <t>EXA Shapes</t>
-  </si>
-  <si>
-    <t>ADB workload</t>
-  </si>
-  <si>
-    <t>VM.Standard2.1</t>
-  </si>
-  <si>
-    <t>ENTERPRISE_EDITION_EXTREME_PERFORMANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.2.0.4 </t>
-  </si>
-  <si>
-    <t>Exadata.Quarter2.92</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>VM.Standard1.1</t>
-  </si>
-  <si>
-    <t>12.1.0.2</t>
-  </si>
-  <si>
-    <t>DSS</t>
-  </si>
-  <si>
-    <t>Exadata.Half2.184</t>
-  </si>
-  <si>
-    <t>BRING_YOUR_OWN_LICENSE</t>
-  </si>
-  <si>
-    <t>UTF8</t>
-  </si>
-  <si>
-    <t>AR8ADOS710</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>VM.Standard1.2</t>
-  </si>
-  <si>
-    <t>12.2.0.1</t>
-  </si>
-  <si>
-    <t>Exadata.Full2.368</t>
-  </si>
-  <si>
-    <t>AR8ADOS720</t>
-  </si>
-  <si>
-    <t>JSON</t>
-  </si>
-  <si>
-    <t>ENTERPRISE_EDITION_HIGH_PERFORMANCE</t>
-  </si>
-  <si>
-    <t>18.0.0.0</t>
-  </si>
-  <si>
-    <t>Exadata.Quarter1.84</t>
-  </si>
-  <si>
-    <t>AR8APTEC715</t>
-  </si>
-  <si>
-    <t>APEX</t>
-  </si>
-  <si>
-    <t>VM.Standard2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.12.0.0 </t>
-  </si>
-  <si>
-    <t>Exadata.Half1.168</t>
-  </si>
-  <si>
-    <t>AR8ARABICMACS</t>
-  </si>
-  <si>
-    <t>VM.Standard1.4</t>
-  </si>
-  <si>
-    <t>18.13.0.0</t>
-  </si>
-  <si>
-    <t>Exadata.Full1.336</t>
-  </si>
-  <si>
-    <t>AR8ASMO8X</t>
-  </si>
-  <si>
-    <t>VM.Standard1.8</t>
-  </si>
-  <si>
-    <t>18.14.0.0</t>
-  </si>
-  <si>
-    <t>Exadata.Base.48</t>
-  </si>
-  <si>
-    <t>AR8ISO8859P6</t>
-  </si>
-  <si>
-    <t>VM.Standard2.8</t>
-  </si>
-  <si>
-    <t>Exadata.Half3.200</t>
-  </si>
-  <si>
-    <t>AR8MSWIN1256</t>
-  </si>
-  <si>
-    <t>VM.Standard2.16</t>
-  </si>
-  <si>
-    <t>19.10.0.0</t>
-  </si>
-  <si>
-    <t>Exadata.Quater3.100</t>
-  </si>
-  <si>
-    <t>AR8MUSSAD768</t>
-  </si>
-  <si>
-    <t>VM.Standard1.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.11.0.0 </t>
-  </si>
-  <si>
-    <t>Exadata.Full3.400</t>
-  </si>
-  <si>
-    <t>AR8NAFITHA711</t>
-  </si>
-  <si>
-    <t>VM.Standard2.24</t>
-  </si>
-  <si>
-    <t>19.12.0.0</t>
-  </si>
-  <si>
-    <t>Exadata X8M-2</t>
-  </si>
-  <si>
-    <t>AR8NAFITHA721</t>
-  </si>
-  <si>
-    <t>BM.DenseIO1.36</t>
-  </si>
-  <si>
-    <t>21.0.0.0</t>
-  </si>
-  <si>
-    <t>Exadata X9M-2</t>
-  </si>
-  <si>
-    <t>AR8SAKHR706</t>
-  </si>
-  <si>
-    <t>21.3.0.0</t>
-  </si>
-  <si>
-    <t>AR8SAKHR707</t>
-  </si>
-  <si>
-    <t>AZ8ISO8859P9E</t>
-  </si>
-  <si>
-    <t>BG8MSWIN</t>
-  </si>
-  <si>
-    <t>BG8PC437S</t>
-  </si>
-  <si>
-    <t>BLT8CP921</t>
-  </si>
-  <si>
-    <t>BLT8ISO8859P13</t>
-  </si>
-  <si>
-    <t>BLT8MSWIN1257</t>
-  </si>
-  <si>
-    <t>BLT8PC775</t>
-  </si>
-  <si>
-    <t>BN8BSCII</t>
-  </si>
-  <si>
-    <t>CDN8PC863</t>
-  </si>
-  <si>
-    <t>CEL8ISO8859P14</t>
-  </si>
-  <si>
-    <t>CL8ISO8859P5</t>
-  </si>
-  <si>
-    <t>CL8ISOIR111</t>
-  </si>
-  <si>
-    <t>CL8KOI8R</t>
-  </si>
-  <si>
-    <t>CL8KOI8U</t>
-  </si>
-  <si>
-    <t>CL8MACCYRILLICS</t>
-  </si>
-  <si>
-    <t>CL8MSWIN1251</t>
-  </si>
-  <si>
-    <t>EE8ISO8859P2</t>
-  </si>
-  <si>
-    <t>EE8MACCES</t>
-  </si>
-  <si>
-    <t>EE8MACCROATIANS</t>
-  </si>
-  <si>
-    <t>EE8MSWIN1250</t>
-  </si>
-  <si>
-    <t>EE8PC852</t>
-  </si>
-  <si>
-    <t>EL8DEC</t>
-  </si>
-  <si>
-    <t>EL8ISO8859P7</t>
-  </si>
-  <si>
-    <t>EL8MACGREEKS</t>
-  </si>
-  <si>
-    <t>EL8MSWIN1253</t>
-  </si>
-  <si>
-    <t>EL8PC437S</t>
-  </si>
-  <si>
-    <t>EL8PC851</t>
-  </si>
-  <si>
-    <t>EL8PC869</t>
-  </si>
-  <si>
-    <t>ET8MSWIN923</t>
-  </si>
-  <si>
-    <t>HU8ABMOD</t>
-  </si>
-  <si>
-    <t>HU8CWI2</t>
-  </si>
-  <si>
-    <t>IN8ISCII</t>
-  </si>
-  <si>
-    <t>IS8PC861</t>
-  </si>
-  <si>
-    <t>IW8ISO8859P8</t>
-  </si>
-  <si>
-    <t>IW8MACHEBREWS</t>
-  </si>
-  <si>
-    <t>IW8MSWIN1255</t>
-  </si>
-  <si>
-    <t>IW8PC1507</t>
-  </si>
-  <si>
-    <t>JA16EUC</t>
-  </si>
-  <si>
-    <t>JA16EUCTILDE</t>
-  </si>
-  <si>
-    <t>JA16SJIS</t>
-  </si>
-  <si>
-    <t>JA16SJISTILDE</t>
-  </si>
-  <si>
-    <t>JA16VMS</t>
-  </si>
-  <si>
-    <t>KO16KSC5601</t>
-  </si>
-  <si>
-    <t>KO16KSCCS</t>
-  </si>
-  <si>
-    <t>KO16MSWIN949</t>
-  </si>
-  <si>
-    <t>LA8ISO6937</t>
-  </si>
-  <si>
-    <t>LA8PASSPORT</t>
-  </si>
-  <si>
-    <t>LT8MSWIN921</t>
-  </si>
-  <si>
-    <t>LT8PC772</t>
-  </si>
-  <si>
-    <t>LT8PC774</t>
-  </si>
-  <si>
-    <t>LV8PC1117</t>
-  </si>
-  <si>
-    <t>LV8PC8LR</t>
-  </si>
-  <si>
-    <t>LV8RST104090</t>
-  </si>
-  <si>
-    <t>N8PC865</t>
-  </si>
-  <si>
-    <t>NE8ISO8859P10</t>
-  </si>
-  <si>
-    <t>NEE8ISO8859P4</t>
-  </si>
-  <si>
-    <t>RU8BESTA</t>
-  </si>
-  <si>
-    <t>RU8PC855</t>
-  </si>
-  <si>
-    <t>RU8PC866</t>
-  </si>
-  <si>
-    <t>SE8ISO8859P3</t>
-  </si>
-  <si>
-    <t>TH8MACTHAIS</t>
-  </si>
-  <si>
-    <t>TH8TISASCII</t>
-  </si>
-  <si>
-    <t>TR8DEC</t>
-  </si>
-  <si>
-    <t>TR8MACTURKISHS</t>
-  </si>
-  <si>
-    <t>TR8MSWIN1254</t>
-  </si>
-  <si>
-    <t>TR8PC857</t>
-  </si>
-  <si>
-    <t>US7ASCII</t>
-  </si>
-  <si>
-    <t>US8PC437</t>
-  </si>
-  <si>
-    <t>VN8MSWIN1258</t>
-  </si>
-  <si>
-    <t>VN8VN3</t>
-  </si>
-  <si>
-    <t>WE8DEC</t>
-  </si>
-  <si>
-    <t>WE8DG</t>
-  </si>
-  <si>
-    <t>WE8ISO8859P1</t>
-  </si>
-  <si>
-    <t>WE8ISO8859P15</t>
-  </si>
-  <si>
-    <t>WE8ISO8859P9</t>
-  </si>
-  <si>
-    <t>WE8MACROMAN8S</t>
-  </si>
-  <si>
-    <t>WE8MSWIN1252</t>
-  </si>
-  <si>
-    <t>WE8NCR4970</t>
-  </si>
-  <si>
-    <t>WE8NEXTSTEP</t>
-  </si>
-  <si>
-    <t>WE8PC850</t>
-  </si>
-  <si>
-    <t>WE8PC858</t>
-  </si>
-  <si>
-    <t>WE8PC860</t>
-  </si>
-  <si>
-    <t>WE8ROMAN8</t>
-  </si>
-  <si>
-    <t>ZHS16CGB231280</t>
-  </si>
-  <si>
-    <t>ZHS16GBK</t>
-  </si>
-  <si>
-    <t>ZHT16BIG5</t>
-  </si>
-  <si>
-    <t>ZHT16CCDC</t>
-  </si>
-  <si>
-    <t>ZHT16DBT</t>
-  </si>
-  <si>
-    <t>ZHT16HKSCS</t>
-  </si>
-  <si>
-    <t>ZHT16MSWIN950</t>
-  </si>
-  <si>
-    <t>ZHT32EUC</t>
-  </si>
-  <si>
-    <t>ZHT32SOPS</t>
-  </si>
-  <si>
-    <t>ZHT32TRIS</t>
-  </si>
-  <si>
-    <r>
-      <t>"Attached To</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" - Valid format:
-VCN::&lt;vcn_name&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Import DRG Route Distribution Statements"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Valid format: &lt;matchtype&gt;::&lt;type|ocid&gt;::&lt;priority&gt;  Multiple statements are seperated by newline in the same cell(\n is not supported)
- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>eg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ALL::::1
-       DRG_ATTACHMENT_TYPE::VCN::2
-       DRG_ATTACHMENT_TYPE::IPSEC_TUNNEL::2
-       DRG_ATTACHMENT_TYPE::REMOTE_PEERING_CONNECTION::2
-       DRG_ATTACHMENT_TYPE::VIRTUAL_CIRCUIT::2
-       DRG_ATTACHMENT_ID::&lt;OCID&gt;::3</t>
-    </r>
+  </si>
+  <si>
+    <t>shell_scriptone</t>
+  </si>
+  <si>
+    <t>ansible_test-script</t>
+  </si>
+  <si>
+    <t>shell_bootstraptscript</t>
+  </si>
+  <si>
+    <t>ansible_testingscript</t>
   </si>
 </sst>
 </file>
@@ -13911,7 +13961,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -26247,10 +26297,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -26264,21 +26314,21 @@
     <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.1796875" customWidth="1"/>
-    <col min="11" max="11" width="14.1796875" customWidth="1"/>
-    <col min="12" max="13" width="20.81640625" customWidth="1"/>
-    <col min="14" max="14" width="21.81640625" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" customWidth="1"/>
-    <col min="17" max="17" width="19" customWidth="1"/>
-    <col min="18" max="18" width="8.36328125" customWidth="1"/>
-    <col min="19" max="19" width="12.1796875" customWidth="1"/>
-    <col min="20" max="20" width="12.81640625" customWidth="1"/>
+    <col min="10" max="11" width="22.1796875" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="14" width="20.81640625" customWidth="1"/>
+    <col min="15" max="15" width="21.81640625" customWidth="1"/>
+    <col min="16" max="16" width="15.6328125" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" customWidth="1"/>
+    <col min="18" max="18" width="19" customWidth="1"/>
+    <col min="19" max="19" width="8.36328125" customWidth="1"/>
+    <col min="20" max="20" width="12.1796875" customWidth="1"/>
+    <col min="21" max="21" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="167.5" customHeight="1">
+    <row r="1" spans="1:21" ht="221" customHeight="1">
       <c r="A1" s="116" t="s">
-        <v>1037</v>
+        <v>1253</v>
       </c>
       <c r="B1" s="117"/>
       <c r="C1" s="117"/>
@@ -26300,9 +26350,10 @@
       <c r="Q1" s="109"/>
       <c r="R1" s="109"/>
       <c r="S1" s="109"/>
-      <c r="T1" s="110"/>
-    </row>
-    <row r="2" spans="1:20" s="44" customFormat="1" ht="52.5" customHeight="1">
+      <c r="T1" s="109"/>
+      <c r="U1" s="110"/>
+    </row>
+    <row r="2" spans="1:21" s="44" customFormat="1" ht="52.5" customHeight="1">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -26334,37 +26385,40 @@
         <v>82</v>
       </c>
       <c r="K2" s="31" t="s">
+        <v>1251</v>
+      </c>
+      <c r="L2" s="31" t="s">
         <v>648</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="M2" s="31" t="s">
         <v>649</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="N2" s="32" t="s">
         <v>652</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="O2" s="32" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="P2" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="Q2" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="R2" s="31" t="s">
+      <c r="S2" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="32" t="s">
+      <c r="T2" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="U2" s="31" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="29">
+    <row r="3" spans="1:21" ht="29">
       <c r="A3" s="37" t="s">
         <v>314</v>
       </c>
@@ -26395,24 +26449,27 @@
       <c r="J3" s="78" t="s">
         <v>948</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="78" t="s">
+        <v>1252</v>
+      </c>
+      <c r="L3" s="37">
         <v>8</v>
       </c>
-      <c r="L3" s="37"/>
       <c r="M3" s="37"/>
       <c r="N3" s="37"/>
-      <c r="O3" s="37" t="s">
+      <c r="O3" s="37"/>
+      <c r="P3" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="37" t="s">
+      <c r="Q3" s="37" t="s">
         <v>575</v>
       </c>
-      <c r="Q3" s="37"/>
       <c r="R3" s="37"/>
       <c r="S3" s="37"/>
       <c r="T3" s="37"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" s="37"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -26430,13 +26487,14 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
-      <c r="P4" s="37"/>
+      <c r="P4" s="9"/>
       <c r="Q4" s="37"/>
-      <c r="R4" s="9"/>
+      <c r="R4" s="37"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="37"/>
-    </row>
-    <row r="5" spans="1:20" ht="58">
+      <c r="T4" s="9"/>
+      <c r="U4" s="37"/>
+    </row>
+    <row r="5" spans="1:21" ht="58">
       <c r="A5" s="53" t="s">
         <v>5</v>
       </c>
@@ -26465,30 +26523,33 @@
       <c r="J5" s="53" t="s">
         <v>331</v>
       </c>
-      <c r="K5" s="53"/>
+      <c r="K5" s="53" t="s">
+        <v>1254</v>
+      </c>
       <c r="L5" s="53"/>
-      <c r="M5" s="53" t="b">
+      <c r="M5" s="53"/>
+      <c r="N5" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53" t="s">
+      <c r="O5" s="53"/>
+      <c r="P5" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="P5" s="53" t="s">
+      <c r="Q5" s="53" t="s">
         <v>435</v>
       </c>
-      <c r="Q5" s="53" t="s">
+      <c r="R5" s="53" t="s">
         <v>351</v>
       </c>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53" t="s">
+      <c r="S5" s="53"/>
+      <c r="T5" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="T5" s="54" t="s">
+      <c r="U5" s="54" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15.5">
+    <row r="6" spans="1:21" ht="15.5">
       <c r="A6" s="53" t="s">
         <v>5</v>
       </c>
@@ -26517,28 +26578,31 @@
       <c r="J6" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="K6" s="84">
+      <c r="K6" s="84" t="s">
+        <v>1255</v>
+      </c>
+      <c r="L6" s="84">
         <v>16</v>
       </c>
-      <c r="L6" s="84">
+      <c r="M6" s="84">
         <v>55</v>
       </c>
-      <c r="M6" s="84"/>
       <c r="N6" s="84"/>
-      <c r="O6" s="53" t="s">
+      <c r="O6" s="84"/>
+      <c r="P6" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="P6" s="53" t="s">
+      <c r="Q6" s="53" t="s">
         <v>376</v>
       </c>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53" t="s">
+      <c r="R6" s="53"/>
+      <c r="S6" s="53" t="s">
         <v>373</v>
       </c>
-      <c r="S6" s="53"/>
       <c r="T6" s="53"/>
-    </row>
-    <row r="7" spans="1:20" ht="15.5">
+      <c r="U6" s="53"/>
+    </row>
+    <row r="7" spans="1:21" ht="15.5">
       <c r="A7" s="53" t="s">
         <v>5</v>
       </c>
@@ -26567,24 +26631,27 @@
       <c r="J7" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="84"/>
+      <c r="K7" s="84" t="s">
+        <v>1256</v>
+      </c>
       <c r="L7" s="84"/>
       <c r="M7" s="84"/>
       <c r="N7" s="84"/>
-      <c r="O7" s="53" t="s">
+      <c r="O7" s="84"/>
+      <c r="P7" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="P7" s="53" t="s">
+      <c r="Q7" s="53" t="s">
         <v>376</v>
       </c>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53" t="s">
+      <c r="R7" s="53"/>
+      <c r="S7" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="S7" s="53"/>
       <c r="T7" s="53"/>
-    </row>
-    <row r="8" spans="1:20" ht="15.5">
+      <c r="U7" s="53"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.5">
       <c r="A8" s="53" t="s">
         <v>5</v>
       </c>
@@ -26613,30 +26680,33 @@
       <c r="J8" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="K8" s="84"/>
+      <c r="K8" s="84" t="s">
+        <v>1257</v>
+      </c>
       <c r="L8" s="84"/>
       <c r="M8" s="84"/>
       <c r="N8" s="84"/>
-      <c r="O8" s="53" t="s">
+      <c r="O8" s="84"/>
+      <c r="P8" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="P8" s="53" t="s">
+      <c r="Q8" s="53" t="s">
         <v>376</v>
       </c>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="53" t="s">
+      <c r="R8" s="53"/>
+      <c r="S8" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="S8" s="53"/>
       <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:T1"/>
+    <mergeCell ref="I1:U1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="P1:Q2 A1:C2 D1:D1048576 R1:XFD1048576 E1:G2 H1:O1048576" xr:uid="{B727580F-A9BA-874F-B6B3-796C3608F9F2}"/>
+    <dataValidation allowBlank="1" sqref="Q1:R2 A1:C2 D1:D1048576 S1:XFD1048576 E1:G2 H1:P1048576" xr:uid="{B727580F-A9BA-874F-B6B3-796C3608F9F2}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26647,7 +26717,7 @@
           <x14:formula1>
             <xm:f>drop_down_rule_comp!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B1048576 Q3:Q1048576</xm:sqref>
+          <xm:sqref>B3:B1048576 R3:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{30FA0D2E-D10A-A343-878C-E48A2407AF2B}">
           <x14:formula1>
@@ -26677,7 +26747,7 @@
           <x14:formula1>
             <xm:f>drop_down_rule_set!$S$2:$S$4</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P1048576</xm:sqref>
+          <xm:sqref>Q3:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{58CABDAC-3EC8-244C-8CC6-62411D89AED8}">
           <x14:formula1>
@@ -41780,19 +41850,19 @@
   <sheetData>
     <row r="1" spans="1:13" ht="43.5">
       <c r="A1" s="101" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B1" s="101" t="s">
         <v>606</v>
       </c>
       <c r="C1" s="102" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D1" s="102" t="s">
         <v>1098</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="E1" s="101" t="s">
         <v>1099</v>
-      </c>
-      <c r="E1" s="101" t="s">
-        <v>1100</v>
       </c>
       <c r="F1" s="103" t="s">
         <v>610</v>
@@ -41813,25 +41883,25 @@
         <v>604</v>
       </c>
       <c r="L1" s="102" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="M1" s="102"/>
     </row>
     <row r="2" spans="1:13" ht="16">
       <c r="A2" s="105" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>1102</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="C2" s="37" t="s">
         <v>1103</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>1104</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>326</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>322</v>
@@ -41846,7 +41916,7 @@
         <v>80</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="K2" s="37">
         <v>1</v>
@@ -41857,34 +41927,34 @@
     </row>
     <row r="3" spans="1:13" ht="16">
       <c r="A3" s="105" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>395</v>
       </c>
       <c r="C3" s="37" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D3" s="37" t="s">
         <v>1108</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="E3" s="37" t="s">
         <v>1109</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="F3" s="37" t="s">
         <v>1110</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="G3" s="106" t="s">
         <v>1111</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="H3" s="37" t="s">
         <v>1112</v>
-      </c>
-      <c r="H3" s="37" t="s">
-        <v>1113</v>
       </c>
       <c r="I3" s="36">
         <v>40</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="K3" s="37">
         <v>2</v>
@@ -41895,24 +41965,24 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="105" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>333</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="37" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F4" s="37"/>
       <c r="H4" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="L4" t="s">
         <v>1118</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -41920,77 +41990,77 @@
         <v>331</v>
       </c>
       <c r="B5" s="37" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C5" s="37" t="s">
         <v>1120</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>1121</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="37" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="F5" s="37"/>
       <c r="H5" s="37" t="s">
+        <v>1122</v>
+      </c>
+      <c r="L5" t="s">
         <v>1123</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="105" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="37" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="37" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F6" s="37"/>
       <c r="H6" s="37" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="105" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="F7" s="37"/>
       <c r="H7" s="37" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="105" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="F8" s="37"/>
       <c r="H8" s="37" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="105" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="37" t="s">
@@ -41998,79 +42068,79 @@
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="F9" s="37"/>
       <c r="H9" s="37" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="105" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="37" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="F10" s="37"/>
       <c r="H10" s="37" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="105" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="37" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F11" s="37"/>
       <c r="H11" s="37" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="105" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="37" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="37" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F12" s="37"/>
       <c r="H12" s="37" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="105" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B13" s="37"/>
       <c r="C13" s="37" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="37" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F13" s="37"/>
       <c r="H13" s="37" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -42079,483 +42149,483 @@
       </c>
       <c r="B14" s="37"/>
       <c r="C14" s="37" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
       <c r="H14" s="37" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="H15" s="37" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="H16" s="37" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="17" spans="8:8">
       <c r="H17" s="37" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="18" spans="8:8">
       <c r="H18" s="37" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="19" spans="8:8">
       <c r="H19" s="37" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="20" spans="8:8">
       <c r="H20" s="37" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="21" spans="8:8">
       <c r="H21" s="37" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="22" spans="8:8">
       <c r="H22" s="37" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="23" spans="8:8">
       <c r="H23" s="37" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="24" spans="8:8">
       <c r="H24" s="37" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="25" spans="8:8">
       <c r="H25" s="37" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="26" spans="8:8">
       <c r="H26" s="37" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="27" spans="8:8">
       <c r="H27" s="37" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="28" spans="8:8">
       <c r="H28" s="37" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="29" spans="8:8">
       <c r="H29" s="37" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="30" spans="8:8">
       <c r="H30" s="37" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="31" spans="8:8">
       <c r="H31" s="37" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="32" spans="8:8">
       <c r="H32" s="37" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="33" spans="8:8">
       <c r="H33" s="37" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="34" spans="8:8">
       <c r="H34" s="37" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="35" spans="8:8">
       <c r="H35" s="37" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="36" spans="8:8">
       <c r="H36" s="37" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="37" spans="8:8">
       <c r="H37" s="37" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="38" spans="8:8">
       <c r="H38" s="37" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="39" spans="8:8">
       <c r="H39" s="37" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="40" spans="8:8">
       <c r="H40" s="37" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="41" spans="8:8">
       <c r="H41" s="37" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="42" spans="8:8">
       <c r="H42" s="37" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="43" spans="8:8">
       <c r="H43" s="37" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="44" spans="8:8">
       <c r="H44" s="37" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="45" spans="8:8">
       <c r="H45" s="37" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="46" spans="8:8">
       <c r="H46" s="37" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="47" spans="8:8">
       <c r="H47" s="37" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="48" spans="8:8">
       <c r="H48" s="37" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="49" spans="8:8">
       <c r="H49" s="37" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="50" spans="8:8">
       <c r="H50" s="37" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="51" spans="8:8">
       <c r="H51" s="37" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="52" spans="8:8">
       <c r="H52" s="37" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="53" spans="8:8">
       <c r="H53" s="37" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="54" spans="8:8">
       <c r="H54" s="37" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="55" spans="8:8">
       <c r="H55" s="37" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="56" spans="8:8">
       <c r="H56" s="37" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="57" spans="8:8">
       <c r="H57" s="37" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="58" spans="8:8">
       <c r="H58" s="37" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="59" spans="8:8">
       <c r="H59" s="37" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="60" spans="8:8">
       <c r="H60" s="37" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="61" spans="8:8">
       <c r="H61" s="37" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="62" spans="8:8">
       <c r="H62" s="37" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="63" spans="8:8">
       <c r="H63" s="37" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="64" spans="8:8">
       <c r="H64" s="37" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="65" spans="8:8">
       <c r="H65" s="37" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="66" spans="8:8">
       <c r="H66" s="37" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="67" spans="8:8">
       <c r="H67" s="37" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="68" spans="8:8">
       <c r="H68" s="37" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="69" spans="8:8">
       <c r="H69" s="37" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="70" spans="8:8">
       <c r="H70" s="37" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="71" spans="8:8">
       <c r="H71" s="37" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="72" spans="8:8">
       <c r="H72" s="37" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="73" spans="8:8">
       <c r="H73" s="37" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="74" spans="8:8">
       <c r="H74" s="37" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="75" spans="8:8">
       <c r="H75" s="37" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="76" spans="8:8">
       <c r="H76" s="37" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="77" spans="8:8">
       <c r="H77" s="37" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="78" spans="8:8">
       <c r="H78" s="37" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="79" spans="8:8">
       <c r="H79" s="37" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="80" spans="8:8">
       <c r="H80" s="37" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="81" spans="8:8">
       <c r="H81" s="37" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="82" spans="8:8">
       <c r="H82" s="37" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="83" spans="8:8">
       <c r="H83" s="37" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="84" spans="8:8">
       <c r="H84" s="37" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="85" spans="8:8">
       <c r="H85" s="37" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="86" spans="8:8">
       <c r="H86" s="37" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="87" spans="8:8">
       <c r="H87" s="37" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="88" spans="8:8">
       <c r="H88" s="37" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="89" spans="8:8">
       <c r="H89" s="37" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="90" spans="8:8">
       <c r="H90" s="37" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="91" spans="8:8">
       <c r="H91" s="37" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="92" spans="8:8">
       <c r="H92" s="37" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="93" spans="8:8">
       <c r="H93" s="37" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="94" spans="8:8">
       <c r="H94" s="37" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="95" spans="8:8">
       <c r="H95" s="37" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="96" spans="8:8">
       <c r="H96" s="37" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="97" spans="8:8">
       <c r="H97" s="37" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="98" spans="8:8">
       <c r="H98" s="37" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="99" spans="8:8">
       <c r="H99" s="37" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="100" spans="8:8">
       <c r="H100" s="37" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="101" spans="8:8">
       <c r="H101" s="37" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="102" spans="8:8">
       <c r="H102" s="37" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="103" spans="8:8">
       <c r="H103" s="37" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="104" spans="8:8">
       <c r="H104" s="37" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="105" spans="8:8">
       <c r="H105" s="37" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="106" spans="8:8">
       <c r="H106" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="107" spans="8:8">
       <c r="H107" s="37" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="108" spans="8:8">
       <c r="H108" s="37" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
   </sheetData>
@@ -43429,7 +43499,7 @@
         <v>497</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
@@ -43441,7 +43511,7 @@
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
       <c r="E4" s="36" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
@@ -43881,7 +43951,7 @@
       <c r="C40" s="36"/>
       <c r="D40" s="36"/>
       <c r="E40" s="36" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
@@ -43893,7 +43963,7 @@
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
       <c r="E41" s="36" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F41" s="36"/>
       <c r="G41" s="36"/>
@@ -43905,7 +43975,7 @@
       <c r="C42" s="36"/>
       <c r="D42" s="36"/>
       <c r="E42" s="36" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
@@ -43917,7 +43987,7 @@
       <c r="C43" s="36"/>
       <c r="D43" s="36"/>
       <c r="E43" s="36" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F43" s="36"/>
       <c r="G43" s="36"/>
@@ -43929,7 +43999,7 @@
       <c r="C44" s="36"/>
       <c r="D44" s="36"/>
       <c r="E44" s="36" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
@@ -43941,7 +44011,7 @@
       <c r="C45" s="36"/>
       <c r="D45" s="36"/>
       <c r="E45" s="36" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
@@ -43961,7 +44031,7 @@
         <v>463</v>
       </c>
       <c r="E46" s="36" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F46" s="36"/>
       <c r="G46" s="36"/>
@@ -43973,7 +44043,7 @@
       <c r="C47" s="36"/>
       <c r="D47" s="36"/>
       <c r="E47" s="36" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F47" s="36"/>
       <c r="G47" s="36"/>
@@ -43985,7 +44055,7 @@
       <c r="C48" s="36"/>
       <c r="D48" s="36"/>
       <c r="E48" s="36" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="F48" s="36"/>
       <c r="G48" s="36"/>
@@ -43997,7 +44067,7 @@
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
       <c r="E49" s="36" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="F49" s="36"/>
       <c r="G49" s="36"/>
@@ -44009,7 +44079,7 @@
       <c r="C50" s="36"/>
       <c r="D50" s="36"/>
       <c r="E50" s="36" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
@@ -44021,7 +44091,7 @@
       <c r="C51" s="36"/>
       <c r="D51" s="36"/>
       <c r="E51" s="36" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F51" s="36"/>
       <c r="G51" s="36"/>
@@ -44033,7 +44103,7 @@
       <c r="C52" s="36"/>
       <c r="D52" s="36"/>
       <c r="E52" s="36" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F52" s="36"/>
       <c r="G52" s="36"/>
@@ -44045,7 +44115,7 @@
       <c r="C53" s="36"/>
       <c r="D53" s="36"/>
       <c r="E53" s="36" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
@@ -44057,7 +44127,7 @@
       <c r="C54" s="36"/>
       <c r="D54" s="36"/>
       <c r="E54" s="36" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F54" s="36"/>
       <c r="G54" s="36"/>
@@ -44069,7 +44139,7 @@
       <c r="C55" s="36"/>
       <c r="D55" s="36"/>
       <c r="E55" s="36" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="F55" s="36"/>
       <c r="G55" s="36"/>
@@ -44081,7 +44151,7 @@
       <c r="C56" s="36"/>
       <c r="D56" s="36"/>
       <c r="E56" s="36" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F56" s="36"/>
       <c r="G56" s="36"/>
@@ -44093,7 +44163,7 @@
       <c r="C57" s="36"/>
       <c r="D57" s="36"/>
       <c r="E57" s="36" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="F57" s="36"/>
       <c r="G57" s="36"/>
@@ -44105,7 +44175,7 @@
       <c r="C58" s="36"/>
       <c r="D58" s="36"/>
       <c r="E58" s="36" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="F58" s="36"/>
       <c r="G58" s="36"/>
@@ -44117,7 +44187,7 @@
       <c r="C59" s="36"/>
       <c r="D59" s="36"/>
       <c r="E59" s="36" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
@@ -44129,7 +44199,7 @@
       <c r="C60" s="36"/>
       <c r="D60" s="36"/>
       <c r="E60" s="36" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F60" s="36"/>
       <c r="G60" s="36"/>
@@ -44141,7 +44211,7 @@
       <c r="C61" s="36"/>
       <c r="D61" s="36"/>
       <c r="E61" s="36" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
@@ -44153,7 +44223,7 @@
       <c r="C62" s="36"/>
       <c r="D62" s="36"/>
       <c r="E62" s="36" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F62" s="36"/>
       <c r="G62" s="36"/>
@@ -44170,10 +44240,10 @@
         <v>384</v>
       </c>
       <c r="D63" s="36" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E63" s="36" t="s">
         <v>1063</v>
-      </c>
-      <c r="E63" s="36" t="s">
-        <v>1064</v>
       </c>
       <c r="F63" s="36"/>
       <c r="G63" s="36"/>
@@ -44185,7 +44255,7 @@
       <c r="C64" s="36"/>
       <c r="D64" s="36"/>
       <c r="E64" s="36" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="F64" s="36"/>
       <c r="G64" s="36"/>
@@ -44197,7 +44267,7 @@
       <c r="C65" s="36"/>
       <c r="D65" s="36"/>
       <c r="E65" s="36" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F65" s="36"/>
       <c r="G65" s="36"/>
@@ -44209,7 +44279,7 @@
       <c r="C66" s="36"/>
       <c r="D66" s="36"/>
       <c r="E66" s="36" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F66" s="36"/>
       <c r="G66" s="36"/>
@@ -44220,7 +44290,7 @@
         <v>5</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>384</v>
@@ -44229,7 +44299,7 @@
         <v>858</v>
       </c>
       <c r="E67" s="36" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F67" s="36"/>
       <c r="G67" s="36"/>
@@ -44241,7 +44311,7 @@
       <c r="C68" s="36"/>
       <c r="D68" s="36"/>
       <c r="E68" s="36" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
@@ -44253,7 +44323,7 @@
       <c r="C69" s="36"/>
       <c r="D69" s="36"/>
       <c r="E69" s="36" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F69" s="36"/>
       <c r="G69" s="36"/>
@@ -44621,7 +44691,7 @@
       <c r="C99" s="36"/>
       <c r="D99" s="36"/>
       <c r="E99" s="36" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="F99" s="36"/>
       <c r="G99" s="36"/>
@@ -44633,7 +44703,7 @@
       <c r="C100" s="36"/>
       <c r="D100" s="36"/>
       <c r="E100" s="36" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="F100" s="36"/>
       <c r="G100" s="36"/>
@@ -44665,7 +44735,7 @@
         <v>466</v>
       </c>
       <c r="E102" s="75" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="F102" s="36"/>
       <c r="G102" s="36"/>
@@ -44677,7 +44747,7 @@
       <c r="C103" s="36"/>
       <c r="D103" s="36"/>
       <c r="E103" s="75" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F103" s="36"/>
       <c r="G103" s="36"/>
@@ -44749,7 +44819,7 @@
       <c r="C109" s="36"/>
       <c r="D109" s="36"/>
       <c r="E109" s="36" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F109" s="36"/>
       <c r="G109" s="36"/>
@@ -45189,7 +45259,7 @@
       <c r="C145" s="36"/>
       <c r="D145" s="36"/>
       <c r="E145" s="36" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F145" s="36"/>
       <c r="G145" s="36"/>
@@ -45201,7 +45271,7 @@
       <c r="C146" s="36"/>
       <c r="D146" s="36"/>
       <c r="E146" s="36" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F146" s="36"/>
       <c r="G146" s="36"/>
@@ -45213,7 +45283,7 @@
       <c r="C147" s="36"/>
       <c r="D147" s="36"/>
       <c r="E147" s="36" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F147" s="36"/>
       <c r="G147" s="36"/>
@@ -45233,7 +45303,7 @@
         <v>499</v>
       </c>
       <c r="E148" s="36" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F148" s="36"/>
       <c r="G148" s="36"/>
@@ -45253,7 +45323,7 @@
         <v>624</v>
       </c>
       <c r="E149" s="100" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="F149" s="36"/>
       <c r="G149" s="36"/>
@@ -45277,7 +45347,7 @@
       <c r="C151" s="36"/>
       <c r="D151" s="36"/>
       <c r="E151" s="36" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F151" s="36"/>
       <c r="G151" s="36"/>
@@ -45289,7 +45359,7 @@
       <c r="C152" s="36"/>
       <c r="D152" s="36"/>
       <c r="E152" s="36" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F152" s="36"/>
       <c r="G152" s="36"/>
@@ -45309,7 +45379,7 @@
         <v>470</v>
       </c>
       <c r="E153" s="36" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F153" s="36"/>
       <c r="G153" s="36"/>
@@ -45321,7 +45391,7 @@
       <c r="C154" s="36"/>
       <c r="D154" s="36"/>
       <c r="E154" s="36" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F154" s="36"/>
       <c r="G154" s="36"/>
@@ -45333,7 +45403,7 @@
       <c r="C155" s="36"/>
       <c r="D155" s="36"/>
       <c r="E155" s="36" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F155" s="36"/>
       <c r="G155" s="36"/>
@@ -45345,7 +45415,7 @@
       <c r="C156" s="36"/>
       <c r="D156" s="36"/>
       <c r="E156" s="36" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="F156" s="36"/>
       <c r="G156" s="36"/>
@@ -45357,7 +45427,7 @@
       <c r="C157" s="36"/>
       <c r="D157" s="36"/>
       <c r="E157" s="36" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="F157" s="36"/>
       <c r="G157" s="36"/>
@@ -45369,7 +45439,7 @@
       <c r="C158" s="36"/>
       <c r="D158" s="36"/>
       <c r="E158" s="36" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="F158" s="36"/>
       <c r="G158" s="36"/>
@@ -45381,7 +45451,7 @@
       <c r="C159" s="36"/>
       <c r="D159" s="36"/>
       <c r="E159" s="36" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="F159" s="36"/>
       <c r="G159" s="36"/>
@@ -45741,7 +45811,7 @@
       <c r="C189" s="36"/>
       <c r="D189" s="36"/>
       <c r="E189" s="36" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="F189" s="36"/>
       <c r="G189" s="36"/>
@@ -45753,7 +45823,7 @@
       <c r="C190" s="36"/>
       <c r="D190" s="36"/>
       <c r="E190" s="36" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="F190" s="36"/>
       <c r="G190" s="36"/>
@@ -45765,7 +45835,7 @@
       <c r="C191" s="36"/>
       <c r="D191" s="36"/>
       <c r="E191" s="36" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="F191" s="36"/>
       <c r="G191" s="36"/>
@@ -45777,7 +45847,7 @@
       <c r="C192" s="36"/>
       <c r="D192" s="36"/>
       <c r="E192" s="36" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F192" s="36"/>
       <c r="G192" s="36"/>
@@ -45789,7 +45859,7 @@
       <c r="C193" s="36"/>
       <c r="D193" s="36"/>
       <c r="E193" s="36" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="F193" s="36"/>
       <c r="G193" s="36"/>
@@ -45801,7 +45871,7 @@
       <c r="C194" s="36"/>
       <c r="D194" s="36"/>
       <c r="E194" s="36" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F194" s="36"/>
       <c r="G194" s="36"/>
@@ -45809,7 +45879,7 @@
     </row>
     <row r="195" spans="1:9" s="37" customFormat="1" ht="29">
       <c r="E195" s="36" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="I195" s="74"/>
     </row>
@@ -46945,7 +47015,7 @@
       <c r="D1" s="107"/>
       <c r="E1" s="107"/>
       <c r="F1" s="114" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="G1" s="114"/>
       <c r="H1" s="114"/>

</xml_diff>

<commit_message>
Automation Toolkit Release v11
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/mycd3/cd3-automation-toolkit/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/cd3devrel/cd3-automation-toolkit/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6FDCC4-BA53-D045-A1D7-D869EC922E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D547F5-9349-A54F-AA2D-205805F09CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -11264,7 +11264,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -11601,7 +11601,6 @@
     <xf numFmtId="0" fontId="35" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -17725,7 +17724,7 @@
       <c r="T14" s="37"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="139" t="s">
+      <c r="A15" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="37"/>
@@ -26941,9 +26940,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" sqref="D1:D2 A1:B2 E1:XFD1048576 C1:C1048576 B3:B1048576" xr:uid="{BB40C8CC-67B2-8947-8DDE-AF0AAC487D9D}"/>
-    <dataValidation allowBlank="1" sqref="D3:D1048576" xr:uid="{6B34CB11-3DA9-1D49-8B26-9BF104EABEBE}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" sqref="A1:B2 B3:B1048576 C1:XFD1048576" xr:uid="{BB40C8CC-67B2-8947-8DDE-AF0AAC487D9D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -55492,20 +55490,15 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" sqref="A1:B2 C1:C1048576 F1:XFD1048576 D1:E2" xr:uid="{A97DD192-90C9-3743-81B1-04F12918A7AB}"/>
+    <dataValidation allowBlank="1" sqref="E3:E1048576" xr:uid="{C42B24AD-BEBE-2C40-944C-813AF6073D75}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{C42B24AD-BEBE-2C40-944C-813AF6073D75}">
-          <x14:formula1>
-            <xm:f>drop_down_rule_set!$B$2:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{211C9B24-9609-374B-A235-F38EBDFE46A0}">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$L$2:$L$44</xm:f>

</xml_diff>

<commit_message>
Revert "Automation Toolkit Release v11"
This reverts commit 10bc8b91f820f8857f35227359f3809b034a24fa.
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/cd3devrel/cd3-automation-toolkit/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/mycd3/cd3-automation-toolkit/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D547F5-9349-A54F-AA2D-205805F09CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6FDCC4-BA53-D045-A1D7-D869EC922E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -11264,7 +11264,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -11601,6 +11601,7 @@
     <xf numFmtId="0" fontId="35" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -17724,7 +17725,7 @@
       <c r="T14" s="37"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="139" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="37"/>
@@ -26940,8 +26941,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="A1:B2 B3:B1048576 C1:XFD1048576" xr:uid="{BB40C8CC-67B2-8947-8DDE-AF0AAC487D9D}"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" sqref="D1:D2 A1:B2 E1:XFD1048576 C1:C1048576 B3:B1048576" xr:uid="{BB40C8CC-67B2-8947-8DDE-AF0AAC487D9D}"/>
+    <dataValidation allowBlank="1" sqref="D3:D1048576" xr:uid="{6B34CB11-3DA9-1D49-8B26-9BF104EABEBE}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -55490,15 +55492,20 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="A1:B2 C1:C1048576 F1:XFD1048576 D1:E2" xr:uid="{A97DD192-90C9-3743-81B1-04F12918A7AB}"/>
-    <dataValidation allowBlank="1" sqref="E3:E1048576" xr:uid="{C42B24AD-BEBE-2C40-944C-813AF6073D75}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{C42B24AD-BEBE-2C40-944C-813AF6073D75}">
+          <x14:formula1>
+            <xm:f>drop_down_rule_set!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{211C9B24-9609-374B-A235-F38EBDFE46A0}">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$L$2:$L$44</xm:f>

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.1.0
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-CIS-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628F8610-7BA1-3C4E-9DC3-3685A1B8EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8461E4D5-2A42-8246-9C4B-A59CFFD797AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="1426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="1427">
   <si>
     <t>Region</t>
   </si>
@@ -10813,6 +10813,9 @@
   </si>
   <si>
     <t>allow any-user to use subnets in compartment Network where all { request.principal.type = 'cluster' }</t>
+  </si>
+  <si>
+    <t>fwl-vcn_fwl-mgmt</t>
   </si>
 </sst>
 </file>
@@ -11471,7 +11474,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -11841,9 +11844,6 @@
     <xf numFmtId="0" fontId="35" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -27317,7 +27317,7 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView showFormulas="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27442,7 +27442,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>314</v>
       </c>
@@ -27459,7 +27459,7 @@
         <v>336</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>582</v>
+        <v>1426</v>
       </c>
       <c r="G3" s="36" t="b">
         <v>0</v>
@@ -55363,7 +55363,7 @@
       <c r="A175" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B175" s="152" t="s">
+      <c r="B175" s="35" t="s">
         <v>452</v>
       </c>
       <c r="C175" s="35" t="s">

</xml_diff>